<commit_message>
Allow for comments field in spreadsheet, plus automatic "I" if "incomplete" is mentioned. Moved grading to a separate tab.
</commit_message>
<xml_diff>
--- a/more-fields-1234.xlsx
+++ b/more-fields-1234.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zives/Python/gradescope-canvas-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B24D9C15-BF8E-AA4F-ADD5-2C1E0C1EE7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E6D208-EA4D-0345-AB87-1D97C77E59DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4460" yWindow="3660" windowWidth="26840" windowHeight="15940" xr2:uid="{44CBF748-CC64-8347-A1BC-8F745DCBB69F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>First Name</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Participation</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Adjustments</t>
   </si>
 </sst>
 </file>
@@ -409,15 +415,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B525A8C4-801C-3C47-982E-88540BE6D4D5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,6 +438,12 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>